<commit_message>
change communication between back and front end
</commit_message>
<xml_diff>
--- a/BackEnd/public/School Curriculums.xlsx
+++ b/BackEnd/public/School Curriculums.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\tablevis\BackEnd\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/runfei/Projects/github/HiTailor/BackEnd/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE05FD3-0EB6-4E32-8FBD-2D61681A0D03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FCF344-9D85-A147-8DD5-A7901A68837D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12132" xr2:uid="{018033FE-E987-497D-8A4E-724D96333FBD}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="12140" xr2:uid="{018033FE-E987-497D-8A4E-724D96333FBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>FALL 2001</t>
   </si>
@@ -103,6 +103,10 @@
   </si>
   <si>
     <t>Sociology</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -113,7 +117,7 @@
     <numFmt numFmtId="176" formatCode="0.0_)"/>
     <numFmt numFmtId="177" formatCode="0_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,10 +205,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -524,44 +528,44 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="16">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="12" t="s">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" ht="16">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -610,11 +614,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="16">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="C3" s="5">
         <v>1083</v>
       </c>
@@ -661,7 +667,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="16">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -712,7 +718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="16">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>11</v>
@@ -763,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="16">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>12</v>
@@ -814,7 +820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="16">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>13</v>
@@ -865,7 +871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="16">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
         <v>14</v>
@@ -916,11 +922,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="16">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="5">
         <v>2113</v>
       </c>
@@ -967,7 +975,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="16">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>16</v>
@@ -1018,7 +1026,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="16">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
         <v>17</v>
@@ -1069,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="16">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>18</v>
@@ -1120,11 +1128,13 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="16">
       <c r="A13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="5">
         <v>3426</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="16">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>20</v>
@@ -1222,7 +1232,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>21</v>
@@ -1273,7 +1283,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>22</v>
@@ -1324,7 +1334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>23</v>
@@ -1375,7 +1385,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>24</v>
@@ -1426,7 +1436,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>25</v>

</xml_diff>